<commit_message>
Added 2 more levels
</commit_message>
<xml_diff>
--- a/Data/Level/Layout_editor.xlsx
+++ b/Data/Level/Layout_editor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog4\Bubble-Bobble\Data\Level\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog4\Bubble-Bobble\Data\Level\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648F8D5E-73A3-4075-B506-0E926C58AC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B90DC4-5D44-46E6-BDAD-225BAD9B0F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13395" yWindow="2745" windowWidth="28800" windowHeight="15885" xr2:uid="{B43FDA53-9266-4FDF-82B6-38A10A7B212D}"/>
+    <workbookView xWindow="20130" yWindow="2655" windowWidth="28800" windowHeight="15885" xr2:uid="{B43FDA53-9266-4FDF-82B6-38A10A7B212D}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
   <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,25 +1740,25 @@
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="1">
         <v>0</v>
@@ -2266,16 +2266,16 @@
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -2287,10 +2287,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
@@ -2311,13 +2311,13 @@
         <v>1</v>
       </c>
       <c r="R13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1">
         <v>1</v>
@@ -2338,10 +2338,10 @@
         <v>1</v>
       </c>
       <c r="AA13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="1">
         <v>0</v>
@@ -2353,16 +2353,16 @@
         <v>0</v>
       </c>
       <c r="AF13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="1">
         <v>1</v>
@@ -2831,16 +2831,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -2918,16 +2918,16 @@
         <v>0</v>
       </c>
       <c r="AF18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ18" s="1">
         <v>1</v>
@@ -3396,25 +3396,25 @@
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -3426,13 +3426,13 @@
         <v>1</v>
       </c>
       <c r="M23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>1</v>
@@ -3456,13 +3456,13 @@
         <v>1</v>
       </c>
       <c r="W23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="1">
         <v>1</v>
@@ -3474,25 +3474,25 @@
         <v>1</v>
       </c>
       <c r="AC23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" s="1">
         <v>1</v>
       </c>
       <c r="AG23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ23" s="1">
         <v>1</v>

</xml_diff>